<commit_message>
lots of discharge data
</commit_message>
<xml_diff>
--- a/Discharge/Discharge_2019/Discharge_Aug01.xlsx
+++ b/Discharge/Discharge_2019/Discharge_Aug01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/LongTermData_CayambeCoca/Discharge/Discharge_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBE589D-77DD-F845-A373-5AE445A6025A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042B97FC-27F4-9D4A-BFB0-A98FD9204E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stn1" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
   <si>
     <t>Station 4</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>New Depth</t>
+  </si>
+  <si>
+    <t>new depth</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1028,7 @@
         <v>4.5760000000000002E-2</v>
       </c>
       <c r="C37">
-        <f t="shared" si="7"/>
+        <f>C23*2.54</f>
         <v>0.17780000000000001</v>
       </c>
       <c r="D37">
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1600,6 +1603,271 @@
       <c r="A31">
         <f>A29-A18</f>
         <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0.7</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>C18*2.54</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>A35</f>
+        <v>0.7</v>
+      </c>
+      <c r="F35">
+        <f>SUM(E35:E53)</f>
+        <v>6.0439807999999977E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0.75</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C46" si="9">C19*2.54</f>
+        <v>2.5400000000000002E-2</v>
+      </c>
+      <c r="D36">
+        <f>(A36+(A37-A36)/2)</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E36">
+        <f>(D36-D35)*(B36)*C36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0.8</v>
+      </c>
+      <c r="B37">
+        <v>0.14872000000000002</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="9"/>
+        <v>5.0800000000000005E-2</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:D38" si="10">(A37+(A38-A37)/2)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="E37">
+        <f>(D37-D36)*(B37)*C37</f>
+        <v>3.7774879999999958E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.85</v>
+      </c>
+      <c r="B38">
+        <v>0.1716</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="9"/>
+        <v>0.127</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="10"/>
+        <v>0.875</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ref="E38:E46" si="11">(D38-D37)*(B38)*C38</f>
+        <v>1.089660000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.9</v>
+      </c>
+      <c r="B39">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="9"/>
+        <v>0.127</v>
+      </c>
+      <c r="D39">
+        <f>(A39+(A40-A39)/2)</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="11"/>
+        <v>5.4483000000000049E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>0.95</v>
+      </c>
+      <c r="B40">
+        <v>8.0079999999999998E-2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="9"/>
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:D46" si="12">(A40+(A41-A40)/2)</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="11"/>
+        <v>6.1020959999999924E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="9"/>
+        <v>0.20320000000000002</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="12"/>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="11"/>
+        <v>5.8115199999999928E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1.05</v>
+      </c>
+      <c r="B42">
+        <v>8.0079999999999998E-2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="9"/>
+        <v>0.2286</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="12"/>
+        <v>1.0750000000000002</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="11"/>
+        <v>9.1531440000000488E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B43">
+        <v>0.10868</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="9"/>
+        <v>0.254</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="12"/>
+        <v>1.125</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="11"/>
+        <v>1.380235999999995E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B44">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="9"/>
+        <v>0.127</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="12"/>
+        <v>1.1749999999999998</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="11"/>
+        <v>5.448299999999981E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1.2</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="9"/>
+        <v>2.5400000000000002E-2</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="12"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1.25</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="12"/>
+        <v>0.625</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +1881,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2373,6 +2641,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BA27023E844F434EBFC790358068B4CE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="962119b939e32e01d6fe84b679c182bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18299441-e87c-4909-bb3a-a1a391a25027" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="185fd3cf949c73c8f7d83010548f2ed9" ns3:_="">
     <xsd:import namespace="18299441-e87c-4909-bb3a-a1a391a25027"/>
@@ -2556,35 +2839,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F37A91D9-9E35-415E-BFF0-EC8FFCDE2D4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98063D7-2718-42E8-A64E-A3E019D8EBDC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18299441-e87c-4909-bb3a-a1a391a25027"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2606,9 +2864,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C98063D7-2718-42E8-A64E-A3E019D8EBDC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F37A91D9-9E35-415E-BFF0-EC8FFCDE2D4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18299441-e87c-4909-bb3a-a1a391a25027"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>